<commit_message>
the Detail of change in description
1. add Assembly-CSharp.csproj To gitignore file;
2. continule finish UI_Bag  module;
3. change BagExcelData class about not inherit MonoBehaviour longer, in other words, i think it couldn't inherit Mono, so what do you think about? Teacher Tuo;
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Data_Bag.xlsx
+++ b/Assets/StreamingAssets/Data_Bag.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="4515" windowHeight="1350"/>
+    <workbookView windowWidth="24000" windowHeight="9765"/>
   </bookViews>
   <sheets>
     <sheet name="Equip" sheetId="5" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="149">
   <si>
     <t>ID</t>
   </si>
@@ -52,6 +52,9 @@
     <t>Price</t>
   </si>
   <si>
+    <t>IsEquip</t>
+  </si>
+  <si>
     <t>Descript</t>
   </si>
   <si>
@@ -89,9 +92,6 @@
   </si>
   <si>
     <t>附魔之锋</t>
-  </si>
-  <si>
-    <t>BOSS掉落</t>
   </si>
   <si>
     <t>附魔的利刃</t>
@@ -604,8 +604,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -618,9 +619,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -641,18 +641,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -665,13 +653,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -689,19 +689,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -725,7 +719,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -749,13 +749,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -767,13 +761,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -791,7 +785,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -809,13 +809,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -932,10 +932,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -944,115 +944,115 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1061,13 +1061,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1403,8 +1403,8 @@
   <sheetPr/>
   <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="N66" sqref="N66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1453,8 +1453,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="O1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -1462,13 +1465,13 @@
         <v>1001</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -1501,7 +1504,7 @@
         <v>0</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -1509,13 +1512,13 @@
         <v>1002</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1">
         <v>3</v>
@@ -1548,7 +1551,7 @@
         <v>0</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -1556,13 +1559,13 @@
         <v>1003</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1">
         <v>5</v>
@@ -1595,7 +1598,7 @@
         <v>0</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1603,13 +1606,13 @@
         <v>1004</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5" s="1">
         <v>7</v>
@@ -1636,13 +1639,13 @@
         <v>0</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N5" s="1">
         <v>0</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -1650,13 +1653,13 @@
         <v>1005</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1">
         <v>10</v>
@@ -1683,10 +1686,10 @@
         <v>0</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>26</v>
@@ -1697,10 +1700,10 @@
         <v>1006</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>27</v>
@@ -1747,7 +1750,7 @@
         <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>31</v>
@@ -1794,7 +1797,7 @@
         <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>33</v>
@@ -1841,7 +1844,7 @@
         <v>30</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>35</v>
@@ -1888,7 +1891,7 @@
         <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>37</v>
@@ -1918,7 +1921,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N11" s="1">
         <v>0</v>
@@ -1935,7 +1938,7 @@
         <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>39</v>
@@ -1965,10 +1968,10 @@
         <v>0</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>40</v>
@@ -1982,7 +1985,7 @@
         <v>30</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>41</v>
@@ -2029,7 +2032,7 @@
         <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>43</v>
@@ -2076,7 +2079,7 @@
         <v>42</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>45</v>
@@ -2123,7 +2126,7 @@
         <v>42</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>47</v>
@@ -2170,7 +2173,7 @@
         <v>42</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>49</v>
@@ -2200,7 +2203,7 @@
         <v>0</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N17" s="1">
         <v>0</v>
@@ -2217,7 +2220,7 @@
         <v>42</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>51</v>
@@ -2247,10 +2250,10 @@
         <v>0</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>52</v>
@@ -2264,7 +2267,7 @@
         <v>42</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>53</v>
@@ -2311,7 +2314,7 @@
         <v>55</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>56</v>
@@ -2358,7 +2361,7 @@
         <v>55</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>58</v>
@@ -2405,7 +2408,7 @@
         <v>55</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>60</v>
@@ -2452,7 +2455,7 @@
         <v>55</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>62</v>
@@ -2482,7 +2485,7 @@
         <v>0</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N23" s="1">
         <v>0</v>
@@ -2499,7 +2502,7 @@
         <v>55</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>64</v>
@@ -2529,10 +2532,10 @@
         <v>0</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="N24" s="1">
+        <v>0</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>65</v>
@@ -2546,7 +2549,7 @@
         <v>55</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>66</v>
@@ -2593,7 +2596,7 @@
         <v>67</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>68</v>
@@ -2640,7 +2643,7 @@
         <v>67</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>70</v>
@@ -2687,7 +2690,7 @@
         <v>67</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>72</v>
@@ -2734,7 +2737,7 @@
         <v>67</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>74</v>
@@ -2764,7 +2767,7 @@
         <v>0</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N29" s="1">
         <v>0</v>
@@ -2781,7 +2784,7 @@
         <v>67</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>76</v>
@@ -2811,10 +2814,10 @@
         <v>0</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N30" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="N30" s="1">
+        <v>0</v>
       </c>
       <c r="O30" s="1" t="s">
         <v>77</v>
@@ -2828,7 +2831,7 @@
         <v>67</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>78</v>
@@ -2875,7 +2878,7 @@
         <v>79</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>80</v>
@@ -2922,7 +2925,7 @@
         <v>79</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>82</v>
@@ -2969,7 +2972,7 @@
         <v>79</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>84</v>
@@ -3016,7 +3019,7 @@
         <v>79</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>86</v>
@@ -3046,7 +3049,7 @@
         <v>0</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N35" s="1">
         <v>0</v>
@@ -3063,7 +3066,7 @@
         <v>79</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>88</v>
@@ -3093,10 +3096,10 @@
         <v>0</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N36" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="N36" s="1">
+        <v>0</v>
       </c>
       <c r="O36" s="1" t="s">
         <v>89</v>
@@ -3110,7 +3113,7 @@
         <v>79</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>90</v>
@@ -3154,7 +3157,7 @@
         <v>1037</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>91</v>
@@ -3201,7 +3204,7 @@
         <v>1038</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>91</v>
@@ -3248,7 +3251,7 @@
         <v>1039</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>91</v>
@@ -3295,7 +3298,7 @@
         <v>1040</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>91</v>
@@ -3328,7 +3331,7 @@
         <v>0</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N41" s="1">
         <v>0</v>
@@ -3342,7 +3345,7 @@
         <v>1041</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>91</v>
@@ -3375,10 +3378,10 @@
         <v>0</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N42" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="N42" s="1">
+        <v>0</v>
       </c>
       <c r="O42" s="1" t="s">
         <v>101</v>
@@ -3389,7 +3392,7 @@
         <v>1042</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>91</v>
@@ -3610,7 +3613,7 @@
         <v>0</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N47" s="1">
         <v>0</v>
@@ -3657,10 +3660,10 @@
         <v>0</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N48" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="N48" s="1">
+        <v>0</v>
       </c>
       <c r="O48" s="1" t="s">
         <v>101</v>
@@ -3892,7 +3895,7 @@
         <v>0</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N53" s="1">
         <v>0</v>
@@ -3939,10 +3942,10 @@
         <v>0</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N54" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="N54" s="1">
+        <v>0</v>
       </c>
       <c r="O54" s="1" t="s">
         <v>101</v>
@@ -4174,7 +4177,7 @@
         <v>0</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N59" s="1">
         <v>0</v>
@@ -4221,10 +4224,10 @@
         <v>0</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N60" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="N60" s="1">
+        <v>0</v>
       </c>
       <c r="O60" s="1" t="s">
         <v>101</v>
@@ -4456,7 +4459,7 @@
         <v>0</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N65" s="1">
         <v>0</v>
@@ -4503,10 +4506,10 @@
         <v>0</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N66" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="N66" s="1">
+        <v>0</v>
       </c>
       <c r="O66" s="1" t="s">
         <v>101</v>
@@ -4738,7 +4741,7 @@
         <v>0</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N71" s="1">
         <v>0</v>
@@ -4785,10 +4788,10 @@
         <v>0</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N72" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="N72" s="1">
+        <v>0</v>
       </c>
       <c r="O72" s="1" t="s">
         <v>101</v>

</xml_diff>